<commit_message>
Completed the readfromexcel page and validated that the date rans as expected, imported the changes to pages checkinfo and login.
</commit_message>
<xml_diff>
--- a/src/test/java/Testdata/data.xlsx
+++ b/src/test/java/Testdata/data.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mihle Matimela\Documents\Automation Course\Assessments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mihle Matimela\Documents\Projects\SauceDemo2ndGroup2025\src\test\java\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:2001_{2F624B92-7C1C-4B25-AF37-9FAF061348CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6BF9191-9471-4F7F-A5CD-30B4341FC7F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23415" yWindow="2910" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{9029EFAD-4DF3-4B15-AA2E-50BF92F45BC4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{9029EFAD-4DF3-4B15-AA2E-50BF92F45BC4}"/>
   </bookViews>
   <sheets>
     <sheet name="Login Details" sheetId="1" r:id="rId1"/>
     <sheet name="User Information" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Username</t>
   </si>
@@ -82,28 +81,34 @@
     <t>secret_sauce1</t>
   </si>
   <si>
-    <t>Information section</t>
-  </si>
-  <si>
-    <t>first-name</t>
-  </si>
-  <si>
-    <t>last-name</t>
-  </si>
-  <si>
-    <t>postal-code</t>
-  </si>
-  <si>
-    <t>User  information</t>
-  </si>
-  <si>
     <t>John</t>
   </si>
   <si>
-    <t>Doe</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Postalcode</t>
+  </si>
+  <si>
+    <t>Lastname</t>
+  </si>
+  <si>
+    <t>Firstname</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>JHRWG</t>
+  </si>
+  <si>
+    <t>Sarah</t>
+  </si>
+  <si>
+    <t>XXXTest</t>
+  </si>
+  <si>
+    <t>ABCDEF</t>
   </si>
 </sst>
 </file>
@@ -119,7 +124,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -135,6 +140,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -166,11 +183,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -188,16 +210,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{08197349-FFB4-47B6-977D-3375CB420327}" name="Table2" displayName="Table2" ref="B2:B5" totalsRowShown="0">
-  <autoFilter ref="B2:B5" xr:uid="{08197349-FFB4-47B6-977D-3375CB420327}"/>
-  <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{CA52EC44-AE2A-491F-806C-02688DC9D32F}" name="User  information"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -520,7 +532,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -628,59 +640,59 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{110EF415-BA76-4F5F-B1DB-7BD8BBD114F2}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
     <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="D1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" t="s">
-        <v>19</v>
+      <c r="B3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="3">
-        <v>12345</v>
-      </c>
+      <c r="B4" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
 </worksheet>
 </file>
</xml_diff>